<commit_message>
project planning: doesn't work
</commit_message>
<xml_diff>
--- a/datafiles/project_planning.xlsx
+++ b/datafiles/project_planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Guest1</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">HG:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The boxes enclosing part of the process
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
@@ -156,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="169" formatCode="[$-14009]d\.m\.yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +213,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -486,11 +534,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,5 +1121,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>